<commit_message>
Added errors and warning messages to test sheets
</commit_message>
<xml_diff>
--- a/module/Import/test/ImportTest/Importer/Nyc/Parser/Excel/_files/class_bad_header.xlsx
+++ b/module/Import/test/ImportTest/Importer/Nyc/Parser/Excel/_files/class_bad_header.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="20540"/>
+    <workbookView xWindow="28740" yWindow="-20060" windowWidth="30500" windowHeight="18760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
+    <sheet name="Errors" sheetId="2" r:id="rId2"/>
+    <sheet name="Warnings" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>8001,8004,8005</t>
   </si>
@@ -45,6 +47,18 @@
   </si>
   <si>
     <t>001</t>
+  </si>
+  <si>
+    <t>'Sheet "Classes" Row: 1 Column "A" in the header is not labeled as "DDBNNN"',</t>
+  </si>
+  <si>
+    <t>'Sheet "Classes" Row: 1 Column "B" in the header is not labeled as "TITLE"',</t>
+  </si>
+  <si>
+    <t>'Sheet "Classes" Row: 1 Column "C" in the header is not labeled as "OFF CLS"',</t>
+  </si>
+  <si>
+    <t>'Sheet "Classes" Row: 1 Column "D" in the header is not labeled as "SUB CLASSES"',</t>
   </si>
 </sst>
 </file>
@@ -412,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -458,4 +472,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="62.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>